<commit_message>
2012-9-26 Sashimi run 49 scripts together.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST1033_ExportLoggedData.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST1033_ExportLoggedData.xlsx
@@ -3743,10 +3743,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RecvDttm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DataLogId</t>
   </si>
   <si>
@@ -3802,6 +3798,10 @@
   </si>
   <si>
     <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecvDttm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4759,8 +4759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4989,16 +4989,16 @@
         <v>796</v>
       </c>
       <c r="I7" s="5" t="s">
+        <v>843</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>844</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>845</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>797</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>798</v>
@@ -5011,7 +5011,7 @@
         <v>765</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C8" s="5">
         <v>7</v>
@@ -5110,7 +5110,7 @@
         <v>56</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -5796,7 +5796,7 @@
         <v>821</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="J36" s="5" t="b">
         <v>1</v>
@@ -5963,7 +5963,7 @@
         <v>43</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>826</v>
@@ -5974,7 +5974,7 @@
         <v>820</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="18"/>
@@ -5999,7 +5999,7 @@
         <v>820</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>828</v>
+        <v>846</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
@@ -6024,7 +6024,7 @@
         <v>820</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
@@ -6049,7 +6049,7 @@
         <v>820</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
@@ -6074,7 +6074,7 @@
         <v>820</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
@@ -6099,7 +6099,7 @@
         <v>820</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
@@ -6124,7 +6124,7 @@
         <v>820</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
@@ -6149,7 +6149,7 @@
         <v>820</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
@@ -6174,7 +6174,7 @@
         <v>820</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
@@ -6199,7 +6199,7 @@
         <v>820</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
@@ -28294,17 +28294,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify some configured ip address and update template for Nancy smoke test.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST1033_ExportLoggedData.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST1033_ExportLoggedData.xlsx
@@ -1209,7 +1209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7393" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7393" uniqueCount="848">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3767,10 +3767,6 @@
     <t>LoggingResult</t>
   </si>
   <si>
-    <t>Fail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3791,17 +3787,27 @@
     <t>2. Timestamp fields will be formatted in the ISO date/time format. And it will be time zone selected in the viewer.</t>
   </si>
   <si>
-    <t>$SNMPdevice_0$</t>
-  </si>
-  <si>
-    <t>$GXT_0_NAME$</t>
-  </si>
-  <si>
     <t>C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RecvDttm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Running Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$SNMP_GXT_0_NAME$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$SNMP_device_0$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contants</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4759,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4945,7 +4951,7 @@
         <v>773</v>
       </c>
       <c r="B6" s="10">
-        <v>41121</v>
+        <v>41450</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
@@ -4989,16 +4995,16 @@
         <v>796</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>797</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>798</v>
@@ -5008,11 +5014,9 @@
     </row>
     <row r="8" spans="1:15" ht="15">
       <c r="A8" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>836</v>
-      </c>
+        <v>844</v>
+      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="5">
         <v>7</v>
       </c>
@@ -5033,11 +5037,9 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>776</v>
-      </c>
+        <v>765</v>
+      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="5">
         <v>8</v>
       </c>
@@ -5063,8 +5065,12 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>776</v>
+      </c>
       <c r="C10" s="5">
         <v>9</v>
       </c>
@@ -5090,10 +5096,8 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="3" t="s">
-        <v>777</v>
-      </c>
-      <c r="B11" s="15"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="5">
         <v>10</v>
       </c>
@@ -5110,7 +5114,7 @@
         <v>56</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -5122,7 +5126,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="5">
@@ -5151,7 +5155,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="5">
@@ -5180,7 +5184,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="5">
@@ -5209,7 +5213,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="5">
@@ -5240,7 +5244,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="5">
@@ -5268,10 +5272,10 @@
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="15" t="s">
-        <v>783</v>
-      </c>
+      <c r="A17" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="5">
         <v>16</v>
       </c>
@@ -5299,7 +5303,7 @@
     <row r="18" spans="1:15">
       <c r="A18" s="3"/>
       <c r="B18" s="15" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C18" s="5">
         <v>17</v>
@@ -5326,11 +5330,9 @@
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="3" t="s">
-        <v>785</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="15" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="C19" s="5">
         <v>18</v>
@@ -5356,9 +5358,11 @@
     </row>
     <row r="20" spans="1:15" ht="15">
       <c r="A20" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="B20" s="15"/>
+        <v>785</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>776</v>
+      </c>
       <c r="C20" s="5">
         <v>19</v>
       </c>
@@ -5379,7 +5383,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="5">
@@ -5407,6 +5411,10 @@
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15">
+      <c r="A22" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="B22" s="15"/>
       <c r="C22" s="5">
         <v>21</v>
       </c>
@@ -5651,7 +5659,7 @@
         <v>809</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>810</v>
+        <v>847</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>819</v>
@@ -5796,7 +5804,7 @@
         <v>821</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="J36" s="5" t="b">
         <v>1</v>
@@ -5963,7 +5971,7 @@
         <v>43</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>826</v>
@@ -5974,9 +5982,11 @@
         <v>820</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>837</v>
-      </c>
-      <c r="J44" s="5"/>
+        <v>836</v>
+      </c>
+      <c r="J44" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K44" s="18"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
@@ -5999,9 +6009,11 @@
         <v>820</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>846</v>
-      </c>
-      <c r="J45" s="5"/>
+        <v>843</v>
+      </c>
+      <c r="J45" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
@@ -6026,7 +6038,9 @@
       <c r="I46" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="J46" s="5"/>
+      <c r="J46" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
@@ -6051,7 +6065,9 @@
       <c r="I47" s="5" t="s">
         <v>829</v>
       </c>
-      <c r="J47" s="5"/>
+      <c r="J47" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
@@ -6076,7 +6092,9 @@
       <c r="I48" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="J48" s="5"/>
+      <c r="J48" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
@@ -6101,7 +6119,9 @@
       <c r="I49" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="J49" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
@@ -6126,7 +6146,9 @@
       <c r="I50" s="5" t="s">
         <v>832</v>
       </c>
-      <c r="J50" s="5"/>
+      <c r="J50" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
@@ -6151,7 +6173,9 @@
       <c r="I51" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="J51" s="5"/>
+      <c r="J51" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
@@ -6176,7 +6200,9 @@
       <c r="I52" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="J52" s="5"/>
+      <c r="J52" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
@@ -6201,7 +6227,9 @@
       <c r="I53" s="5" t="s">
         <v>835</v>
       </c>
-      <c r="J53" s="5"/>
+      <c r="J53" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
@@ -28294,17 +28322,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
   </sheetData>

</xml_diff>